<commit_message>
commit for hw 7 (data prep)
</commit_message>
<xml_diff>
--- a/data_prep.xlsx
+++ b/data_prep.xlsx
@@ -415,8 +415,10 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2">
-        <v>1</v>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
       <c r="B2">
         <v>52</v>
@@ -450,8 +452,10 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3">
-        <v>1</v>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
       <c r="B3">
         <v>37</v>
@@ -485,8 +489,10 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4">
-        <v>1</v>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
       <c r="B4">
         <v>55</v>
@@ -520,8 +526,10 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5">
-        <v>1</v>
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
       <c r="B5">
         <v>42</v>
@@ -555,8 +563,10 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6">
-        <v>1</v>
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
       <c r="B6">
         <v>53</v>
@@ -590,8 +600,10 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7">
-        <v>1</v>
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
       <c r="B7">
         <v>42</v>
@@ -625,8 +637,10 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8">
-        <v>1</v>
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
       <c r="B8">
         <v>53</v>
@@ -660,8 +674,10 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9">
-        <v>1</v>
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
       <c r="B9">
         <v>40</v>
@@ -695,8 +711,10 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10">
-        <v>1</v>
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
       <c r="B10">
         <v>51</v>
@@ -730,8 +748,10 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11">
-        <v>1</v>
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
       <c r="B11">
         <v>43</v>
@@ -765,8 +785,10 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12">
-        <v>1</v>
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
       <c r="B12">
         <v>37</v>
@@ -800,8 +822,10 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13">
-        <v>1</v>
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
       <c r="B13">
         <v>39</v>
@@ -835,8 +859,10 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14">
-        <v>1</v>
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
       <c r="B14">
         <v>39</v>
@@ -870,8 +896,10 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15">
-        <v>1</v>
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
       <c r="B15">
         <v>49</v>
@@ -905,8 +933,10 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16">
-        <v>1</v>
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
       <c r="B16">
         <v>56</v>
@@ -940,8 +970,10 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17">
-        <v>1</v>
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
       <c r="B17">
         <v>43</v>
@@ -975,8 +1007,10 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18">
-        <v>1</v>
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
       <c r="B18">
         <v>40</v>
@@ -1010,8 +1044,10 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19">
-        <v>1</v>
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
       <c r="B19">
         <v>43</v>
@@ -1045,8 +1081,10 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20">
-        <v>1</v>
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
       <c r="B20">
         <v>42</v>
@@ -1080,8 +1118,10 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21">
-        <v>1</v>
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
       <c r="B21">
         <v>50</v>
@@ -1115,8 +1155,10 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22">
-        <v>1</v>
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
       <c r="B22">
         <v>46</v>
@@ -1150,8 +1192,10 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23">
-        <v>1</v>
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
       <c r="B23">
         <v>50</v>
@@ -1185,8 +1229,10 @@
       </c>
     </row>
     <row r="24">
-      <c r="A24">
-        <v>1</v>
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
       <c r="B24">
         <v>52</v>
@@ -1220,8 +1266,10 @@
       </c>
     </row>
     <row r="25">
-      <c r="A25">
-        <v>1</v>
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
       <c r="B25">
         <v>40</v>
@@ -1255,8 +1303,10 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26">
-        <v>1</v>
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
       <c r="B26">
         <v>57</v>
@@ -1290,8 +1340,10 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27">
-        <v>1</v>
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
       <c r="B27">
         <v>41</v>
@@ -1325,8 +1377,10 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28">
-        <v>1</v>
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
       <c r="B28">
         <v>47</v>
@@ -1360,8 +1414,10 @@
       </c>
     </row>
     <row r="29">
-      <c r="A29">
-        <v>1</v>
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
       <c r="B29">
         <v>40</v>
@@ -1395,8 +1451,10 @@
       </c>
     </row>
     <row r="30">
-      <c r="A30">
-        <v>1</v>
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
       <c r="B30">
         <v>50</v>
@@ -1430,8 +1488,10 @@
       </c>
     </row>
     <row r="31">
-      <c r="A31">
-        <v>1</v>
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
       <c r="B31">
         <v>59</v>
@@ -1465,8 +1525,10 @@
       </c>
     </row>
     <row r="32">
-      <c r="A32">
-        <v>2</v>
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
       <c r="B32">
         <v>54</v>
@@ -1500,8 +1562,10 @@
       </c>
     </row>
     <row r="33">
-      <c r="A33">
-        <v>2</v>
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
       <c r="B33">
         <v>52</v>
@@ -1535,8 +1599,10 @@
       </c>
     </row>
     <row r="34">
-      <c r="A34">
-        <v>2</v>
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
       <c r="B34">
         <v>41</v>
@@ -1570,8 +1636,10 @@
       </c>
     </row>
     <row r="35">
-      <c r="A35">
-        <v>2</v>
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
       <c r="B35">
         <v>51</v>
@@ -1605,8 +1673,10 @@
       </c>
     </row>
     <row r="36">
-      <c r="A36">
-        <v>2</v>
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
       <c r="B36">
         <v>38</v>
@@ -1640,8 +1710,10 @@
       </c>
     </row>
     <row r="37">
-      <c r="A37">
-        <v>2</v>
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
       <c r="B37">
         <v>39</v>
@@ -1675,8 +1747,10 @@
       </c>
     </row>
     <row r="38">
-      <c r="A38">
-        <v>2</v>
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
       <c r="B38">
         <v>47</v>
@@ -1710,8 +1784,10 @@
       </c>
     </row>
     <row r="39">
-      <c r="A39">
-        <v>2</v>
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
       <c r="B39">
         <v>50</v>
@@ -1745,8 +1821,10 @@
       </c>
     </row>
     <row r="40">
-      <c r="A40">
-        <v>2</v>
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
       <c r="B40">
         <v>54</v>
@@ -1780,8 +1858,10 @@
       </c>
     </row>
     <row r="41">
-      <c r="A41">
-        <v>2</v>
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
       <c r="B41">
         <v>58</v>
@@ -1815,8 +1895,10 @@
       </c>
     </row>
     <row r="42">
-      <c r="A42">
-        <v>2</v>
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
       <c r="B42">
         <v>46</v>
@@ -1850,8 +1932,10 @@
       </c>
     </row>
     <row r="43">
-      <c r="A43">
-        <v>2</v>
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
       <c r="B43">
         <v>52</v>
@@ -1885,8 +1969,10 @@
       </c>
     </row>
     <row r="44">
-      <c r="A44">
-        <v>2</v>
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
       <c r="B44">
         <v>37</v>
@@ -1920,8 +2006,10 @@
       </c>
     </row>
     <row r="45">
-      <c r="A45">
-        <v>2</v>
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
       <c r="B45">
         <v>55</v>
@@ -1955,8 +2043,10 @@
       </c>
     </row>
     <row r="46">
-      <c r="A46">
-        <v>2</v>
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
       <c r="B46">
         <v>50</v>
@@ -1990,8 +2080,10 @@
       </c>
     </row>
     <row r="47">
-      <c r="A47">
-        <v>2</v>
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
       <c r="B47">
         <v>50</v>
@@ -2025,8 +2117,10 @@
       </c>
     </row>
     <row r="48">
-      <c r="A48">
-        <v>2</v>
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
       <c r="B48">
         <v>37</v>
@@ -2060,8 +2154,10 @@
       </c>
     </row>
     <row r="49">
-      <c r="A49">
-        <v>2</v>
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
       <c r="B49">
         <v>42</v>
@@ -2095,8 +2191,10 @@
       </c>
     </row>
     <row r="50">
-      <c r="A50">
-        <v>2</v>
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
       <c r="B50">
         <v>39</v>
@@ -2130,8 +2228,10 @@
       </c>
     </row>
     <row r="51">
-      <c r="A51">
-        <v>2</v>
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
       <c r="B51">
         <v>42</v>
@@ -2165,8 +2265,10 @@
       </c>
     </row>
     <row r="52">
-      <c r="A52">
-        <v>2</v>
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
       <c r="B52">
         <v>44</v>
@@ -2200,8 +2302,10 @@
       </c>
     </row>
     <row r="53">
-      <c r="A53">
-        <v>2</v>
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
       <c r="B53">
         <v>46</v>
@@ -2235,8 +2339,10 @@
       </c>
     </row>
     <row r="54">
-      <c r="A54">
-        <v>2</v>
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
       <c r="B54">
         <v>49</v>
@@ -2270,8 +2376,10 @@
       </c>
     </row>
     <row r="55">
-      <c r="A55">
-        <v>2</v>
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
       <c r="B55">
         <v>45</v>
@@ -2305,8 +2413,10 @@
       </c>
     </row>
     <row r="56">
-      <c r="A56">
-        <v>2</v>
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
       <c r="B56">
         <v>44</v>
@@ -2340,8 +2450,10 @@
       </c>
     </row>
     <row r="57">
-      <c r="A57">
-        <v>2</v>
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
       <c r="B57">
         <v>40</v>
@@ -2375,8 +2487,10 @@
       </c>
     </row>
     <row r="58">
-      <c r="A58">
-        <v>2</v>
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
       <c r="B58">
         <v>40</v>
@@ -2410,8 +2524,10 @@
       </c>
     </row>
     <row r="59">
-      <c r="A59">
-        <v>2</v>
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
       <c r="B59">
         <v>51</v>
@@ -2445,8 +2561,10 @@
       </c>
     </row>
     <row r="60">
-      <c r="A60">
-        <v>2</v>
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
       <c r="B60">
         <v>42</v>
@@ -2480,8 +2598,10 @@
       </c>
     </row>
     <row r="61">
-      <c r="A61">
-        <v>2</v>
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
       <c r="B61">
         <v>40</v>
@@ -2515,8 +2635,10 @@
       </c>
     </row>
     <row r="62">
-      <c r="A62">
-        <v>2</v>
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
       <c r="B62">
         <v>47</v>
@@ -2550,8 +2672,10 @@
       </c>
     </row>
     <row r="63">
-      <c r="A63">
-        <v>2</v>
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
       <c r="B63">
         <v>40</v>
@@ -2585,8 +2709,10 @@
       </c>
     </row>
     <row r="64">
-      <c r="A64">
-        <v>2</v>
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
       <c r="B64">
         <v>42</v>
@@ -2620,8 +2746,10 @@
       </c>
     </row>
     <row r="65">
-      <c r="A65">
-        <v>2</v>
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
       <c r="B65">
         <v>50</v>
@@ -2655,8 +2783,10 @@
       </c>
     </row>
     <row r="66">
-      <c r="A66">
-        <v>2</v>
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
       <c r="B66">
         <v>50</v>
@@ -2690,8 +2820,10 @@
       </c>
     </row>
     <row r="67">
-      <c r="A67">
-        <v>2</v>
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
       <c r="B67">
         <v>53</v>

</xml_diff>

<commit_message>
commit for hw 8 (starwars) @nrdowling @ysh627
</commit_message>
<xml_diff>
--- a/data_prep.xlsx
+++ b/data_prep.xlsx
@@ -415,10 +415,8 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A2">
+        <v>1</v>
       </c>
       <c r="B2">
         <v>52</v>
@@ -452,10 +450,8 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A3">
+        <v>1</v>
       </c>
       <c r="B3">
         <v>37</v>
@@ -489,10 +485,8 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A4">
+        <v>1</v>
       </c>
       <c r="B4">
         <v>55</v>
@@ -526,10 +520,8 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A5">
+        <v>1</v>
       </c>
       <c r="B5">
         <v>42</v>
@@ -563,10 +555,8 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A6">
+        <v>1</v>
       </c>
       <c r="B6">
         <v>53</v>
@@ -600,10 +590,8 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A7">
+        <v>1</v>
       </c>
       <c r="B7">
         <v>42</v>
@@ -637,10 +625,8 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A8">
+        <v>1</v>
       </c>
       <c r="B8">
         <v>53</v>
@@ -674,10 +660,8 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A9">
+        <v>1</v>
       </c>
       <c r="B9">
         <v>40</v>
@@ -711,10 +695,8 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A10">
+        <v>1</v>
       </c>
       <c r="B10">
         <v>51</v>
@@ -748,10 +730,8 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A11">
+        <v>1</v>
       </c>
       <c r="B11">
         <v>43</v>
@@ -785,10 +765,8 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A12">
+        <v>1</v>
       </c>
       <c r="B12">
         <v>37</v>
@@ -822,10 +800,8 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A13">
+        <v>1</v>
       </c>
       <c r="B13">
         <v>39</v>
@@ -859,10 +835,8 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A14">
+        <v>1</v>
       </c>
       <c r="B14">
         <v>39</v>
@@ -896,10 +870,8 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A15">
+        <v>1</v>
       </c>
       <c r="B15">
         <v>49</v>
@@ -933,10 +905,8 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A16">
+        <v>1</v>
       </c>
       <c r="B16">
         <v>56</v>
@@ -970,10 +940,8 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A17">
+        <v>1</v>
       </c>
       <c r="B17">
         <v>43</v>
@@ -1007,10 +975,8 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A18">
+        <v>1</v>
       </c>
       <c r="B18">
         <v>40</v>
@@ -1044,10 +1010,8 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A19">
+        <v>1</v>
       </c>
       <c r="B19">
         <v>43</v>
@@ -1081,10 +1045,8 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A20">
+        <v>1</v>
       </c>
       <c r="B20">
         <v>42</v>
@@ -1118,10 +1080,8 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A21">
+        <v>1</v>
       </c>
       <c r="B21">
         <v>50</v>
@@ -1155,10 +1115,8 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A22">
+        <v>1</v>
       </c>
       <c r="B22">
         <v>46</v>
@@ -1192,10 +1150,8 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A23">
+        <v>1</v>
       </c>
       <c r="B23">
         <v>50</v>
@@ -1229,10 +1185,8 @@
       </c>
     </row>
     <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A24">
+        <v>1</v>
       </c>
       <c r="B24">
         <v>52</v>
@@ -1266,10 +1220,8 @@
       </c>
     </row>
     <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A25">
+        <v>1</v>
       </c>
       <c r="B25">
         <v>40</v>
@@ -1303,10 +1255,8 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A26">
+        <v>1</v>
       </c>
       <c r="B26">
         <v>57</v>
@@ -1340,10 +1290,8 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A27">
+        <v>1</v>
       </c>
       <c r="B27">
         <v>41</v>
@@ -1377,10 +1325,8 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A28">
+        <v>1</v>
       </c>
       <c r="B28">
         <v>47</v>
@@ -1414,10 +1360,8 @@
       </c>
     </row>
     <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A29">
+        <v>1</v>
       </c>
       <c r="B29">
         <v>40</v>
@@ -1451,10 +1395,8 @@
       </c>
     </row>
     <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A30">
+        <v>1</v>
       </c>
       <c r="B30">
         <v>50</v>
@@ -1488,10 +1430,8 @@
       </c>
     </row>
     <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A31">
+        <v>1</v>
       </c>
       <c r="B31">
         <v>59</v>
@@ -1525,10 +1465,8 @@
       </c>
     </row>
     <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="A32">
+        <v>2</v>
       </c>
       <c r="B32">
         <v>54</v>
@@ -1562,10 +1500,8 @@
       </c>
     </row>
     <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="A33">
+        <v>2</v>
       </c>
       <c r="B33">
         <v>52</v>
@@ -1599,10 +1535,8 @@
       </c>
     </row>
     <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="A34">
+        <v>2</v>
       </c>
       <c r="B34">
         <v>41</v>
@@ -1636,10 +1570,8 @@
       </c>
     </row>
     <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="A35">
+        <v>2</v>
       </c>
       <c r="B35">
         <v>51</v>
@@ -1673,10 +1605,8 @@
       </c>
     </row>
     <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="A36">
+        <v>2</v>
       </c>
       <c r="B36">
         <v>38</v>
@@ -1710,10 +1640,8 @@
       </c>
     </row>
     <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="A37">
+        <v>2</v>
       </c>
       <c r="B37">
         <v>39</v>
@@ -1747,10 +1675,8 @@
       </c>
     </row>
     <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="A38">
+        <v>2</v>
       </c>
       <c r="B38">
         <v>47</v>
@@ -1784,10 +1710,8 @@
       </c>
     </row>
     <row r="39">
-      <c r="A39" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="A39">
+        <v>2</v>
       </c>
       <c r="B39">
         <v>50</v>
@@ -1821,10 +1745,8 @@
       </c>
     </row>
     <row r="40">
-      <c r="A40" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="A40">
+        <v>2</v>
       </c>
       <c r="B40">
         <v>54</v>
@@ -1858,10 +1780,8 @@
       </c>
     </row>
     <row r="41">
-      <c r="A41" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="A41">
+        <v>2</v>
       </c>
       <c r="B41">
         <v>58</v>
@@ -1895,10 +1815,8 @@
       </c>
     </row>
     <row r="42">
-      <c r="A42" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="A42">
+        <v>2</v>
       </c>
       <c r="B42">
         <v>46</v>
@@ -1932,10 +1850,8 @@
       </c>
     </row>
     <row r="43">
-      <c r="A43" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="A43">
+        <v>2</v>
       </c>
       <c r="B43">
         <v>52</v>
@@ -1969,10 +1885,8 @@
       </c>
     </row>
     <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="A44">
+        <v>2</v>
       </c>
       <c r="B44">
         <v>37</v>
@@ -2006,10 +1920,8 @@
       </c>
     </row>
     <row r="45">
-      <c r="A45" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="A45">
+        <v>2</v>
       </c>
       <c r="B45">
         <v>55</v>
@@ -2043,10 +1955,8 @@
       </c>
     </row>
     <row r="46">
-      <c r="A46" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="A46">
+        <v>2</v>
       </c>
       <c r="B46">
         <v>50</v>
@@ -2080,10 +1990,8 @@
       </c>
     </row>
     <row r="47">
-      <c r="A47" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="A47">
+        <v>2</v>
       </c>
       <c r="B47">
         <v>50</v>
@@ -2117,10 +2025,8 @@
       </c>
     </row>
     <row r="48">
-      <c r="A48" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="A48">
+        <v>2</v>
       </c>
       <c r="B48">
         <v>37</v>
@@ -2154,10 +2060,8 @@
       </c>
     </row>
     <row r="49">
-      <c r="A49" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="A49">
+        <v>2</v>
       </c>
       <c r="B49">
         <v>42</v>
@@ -2191,10 +2095,8 @@
       </c>
     </row>
     <row r="50">
-      <c r="A50" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="A50">
+        <v>2</v>
       </c>
       <c r="B50">
         <v>39</v>
@@ -2228,10 +2130,8 @@
       </c>
     </row>
     <row r="51">
-      <c r="A51" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="A51">
+        <v>2</v>
       </c>
       <c r="B51">
         <v>42</v>
@@ -2265,10 +2165,8 @@
       </c>
     </row>
     <row r="52">
-      <c r="A52" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="A52">
+        <v>2</v>
       </c>
       <c r="B52">
         <v>44</v>
@@ -2302,10 +2200,8 @@
       </c>
     </row>
     <row r="53">
-      <c r="A53" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="A53">
+        <v>2</v>
       </c>
       <c r="B53">
         <v>46</v>
@@ -2339,10 +2235,8 @@
       </c>
     </row>
     <row r="54">
-      <c r="A54" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="A54">
+        <v>2</v>
       </c>
       <c r="B54">
         <v>49</v>
@@ -2376,10 +2270,8 @@
       </c>
     </row>
     <row r="55">
-      <c r="A55" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="A55">
+        <v>2</v>
       </c>
       <c r="B55">
         <v>45</v>
@@ -2413,10 +2305,8 @@
       </c>
     </row>
     <row r="56">
-      <c r="A56" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="A56">
+        <v>2</v>
       </c>
       <c r="B56">
         <v>44</v>
@@ -2450,10 +2340,8 @@
       </c>
     </row>
     <row r="57">
-      <c r="A57" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="A57">
+        <v>2</v>
       </c>
       <c r="B57">
         <v>40</v>
@@ -2487,10 +2375,8 @@
       </c>
     </row>
     <row r="58">
-      <c r="A58" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="A58">
+        <v>2</v>
       </c>
       <c r="B58">
         <v>40</v>
@@ -2524,10 +2410,8 @@
       </c>
     </row>
     <row r="59">
-      <c r="A59" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="A59">
+        <v>2</v>
       </c>
       <c r="B59">
         <v>51</v>
@@ -2561,10 +2445,8 @@
       </c>
     </row>
     <row r="60">
-      <c r="A60" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="A60">
+        <v>2</v>
       </c>
       <c r="B60">
         <v>42</v>
@@ -2598,10 +2480,8 @@
       </c>
     </row>
     <row r="61">
-      <c r="A61" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="A61">
+        <v>2</v>
       </c>
       <c r="B61">
         <v>40</v>
@@ -2635,10 +2515,8 @@
       </c>
     </row>
     <row r="62">
-      <c r="A62" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="A62">
+        <v>2</v>
       </c>
       <c r="B62">
         <v>47</v>
@@ -2672,10 +2550,8 @@
       </c>
     </row>
     <row r="63">
-      <c r="A63" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="A63">
+        <v>2</v>
       </c>
       <c r="B63">
         <v>40</v>
@@ -2709,10 +2585,8 @@
       </c>
     </row>
     <row r="64">
-      <c r="A64" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="A64">
+        <v>2</v>
       </c>
       <c r="B64">
         <v>42</v>
@@ -2746,10 +2620,8 @@
       </c>
     </row>
     <row r="65">
-      <c r="A65" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="A65">
+        <v>2</v>
       </c>
       <c r="B65">
         <v>50</v>
@@ -2783,10 +2655,8 @@
       </c>
     </row>
     <row r="66">
-      <c r="A66" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="A66">
+        <v>2</v>
       </c>
       <c r="B66">
         <v>50</v>
@@ -2820,10 +2690,8 @@
       </c>
     </row>
     <row r="67">
-      <c r="A67" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="A67">
+        <v>2</v>
       </c>
       <c r="B67">
         <v>53</v>

</xml_diff>

<commit_message>
commit for hw 20 @nrdowling @ysh627
</commit_message>
<xml_diff>
--- a/data_prep.xlsx
+++ b/data_prep.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K67"/>
+  <dimension ref="A1:J67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -360,7 +360,7 @@
     <row r="1" s="1" customFormat="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>social_class</t>
+          <t>vignette_type</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -380,35 +380,30 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>perceived_comp</t>
+          <t>infer_knowledge</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>perceived_intel</t>
+          <t>topic_knowledge</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>hiring_pref</t>
+          <t>evaluator_gender</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>evaluator_gender</t>
+          <t>evaluator_age</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>evaluator_age</t>
+          <t>evaluator_edu</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>evaluator_edu</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>evaluator_class</t>
         </is>
@@ -417,7 +412,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>upper-class</t>
+          <t>higher-class</t>
         </is>
       </c>
       <c r="B2">
@@ -435,28 +430,25 @@
       <c r="F2">
         <v>3</v>
       </c>
-      <c r="G2">
-        <v>3</v>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>male</t>
-        </is>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>male</t>
+        </is>
+      </c>
+      <c r="H2">
+        <v>52</v>
       </c>
       <c r="I2">
-        <v>52</v>
+        <v>6</v>
       </c>
       <c r="J2">
-        <v>6</v>
-      </c>
-      <c r="K2">
         <v>4</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>upper-class</t>
+          <t>higher-class</t>
         </is>
       </c>
       <c r="B3">
@@ -474,28 +466,25 @@
       <c r="F3">
         <v>3</v>
       </c>
-      <c r="G3">
-        <v>2</v>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>female</t>
-        </is>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>female</t>
+        </is>
+      </c>
+      <c r="H3">
+        <v>37</v>
       </c>
       <c r="I3">
-        <v>37</v>
+        <v>5</v>
       </c>
       <c r="J3">
-        <v>5</v>
-      </c>
-      <c r="K3">
         <v>4</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>upper-class</t>
+          <t>higher-class</t>
         </is>
       </c>
       <c r="B4">
@@ -513,28 +502,25 @@
       <c r="F4">
         <v>4</v>
       </c>
-      <c r="G4">
-        <v>4</v>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>male</t>
-        </is>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>male</t>
+        </is>
+      </c>
+      <c r="H4">
+        <v>55</v>
       </c>
       <c r="I4">
-        <v>55</v>
+        <v>5</v>
       </c>
       <c r="J4">
-        <v>5</v>
-      </c>
-      <c r="K4">
         <v>5</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>upper-class</t>
+          <t>higher-class</t>
         </is>
       </c>
       <c r="B5">
@@ -552,28 +538,25 @@
       <c r="F5">
         <v>3</v>
       </c>
-      <c r="G5">
-        <v>3</v>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>female</t>
-        </is>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>female</t>
+        </is>
+      </c>
+      <c r="H5">
+        <v>42</v>
       </c>
       <c r="I5">
-        <v>42</v>
+        <v>4</v>
       </c>
       <c r="J5">
-        <v>4</v>
-      </c>
-      <c r="K5">
         <v>5</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>upper-class</t>
+          <t>higher-class</t>
         </is>
       </c>
       <c r="B6">
@@ -586,33 +569,30 @@
         <v>7</v>
       </c>
       <c r="E6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F6">
         <v>3</v>
       </c>
-      <c r="G6">
-        <v>4</v>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>male</t>
-        </is>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>male</t>
+        </is>
+      </c>
+      <c r="H6">
+        <v>53</v>
       </c>
       <c r="I6">
-        <v>53</v>
+        <v>5</v>
       </c>
       <c r="J6">
-        <v>5</v>
-      </c>
-      <c r="K6">
         <v>7</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>upper-class</t>
+          <t>higher-class</t>
         </is>
       </c>
       <c r="B7">
@@ -630,28 +610,25 @@
       <c r="F7">
         <v>3</v>
       </c>
-      <c r="G7">
-        <v>3</v>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>male</t>
-        </is>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>male</t>
+        </is>
+      </c>
+      <c r="H7">
+        <v>42</v>
       </c>
       <c r="I7">
-        <v>42</v>
+        <v>4</v>
       </c>
       <c r="J7">
-        <v>4</v>
-      </c>
-      <c r="K7">
         <v>5</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>upper-class</t>
+          <t>higher-class</t>
         </is>
       </c>
       <c r="B8">
@@ -669,28 +646,25 @@
       <c r="F8">
         <v>4</v>
       </c>
-      <c r="G8">
-        <v>5</v>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>male</t>
-        </is>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>male</t>
+        </is>
+      </c>
+      <c r="H8">
+        <v>53</v>
       </c>
       <c r="I8">
-        <v>53</v>
+        <v>5</v>
       </c>
       <c r="J8">
-        <v>5</v>
-      </c>
-      <c r="K8">
         <v>3</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>upper-class</t>
+          <t>higher-class</t>
         </is>
       </c>
       <c r="B9">
@@ -708,28 +682,25 @@
       <c r="F9">
         <v>3</v>
       </c>
-      <c r="G9">
-        <v>3</v>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>female</t>
-        </is>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>female</t>
+        </is>
+      </c>
+      <c r="H9">
+        <v>40</v>
       </c>
       <c r="I9">
-        <v>40</v>
+        <v>5</v>
       </c>
       <c r="J9">
-        <v>5</v>
-      </c>
-      <c r="K9">
         <v>4</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>upper-class</t>
+          <t>higher-class</t>
         </is>
       </c>
       <c r="B10">
@@ -747,28 +718,25 @@
       <c r="F10">
         <v>4</v>
       </c>
-      <c r="G10">
-        <v>2</v>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>male</t>
-        </is>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>male</t>
+        </is>
+      </c>
+      <c r="H10">
+        <v>51</v>
       </c>
       <c r="I10">
-        <v>51</v>
+        <v>5</v>
       </c>
       <c r="J10">
-        <v>5</v>
-      </c>
-      <c r="K10">
         <v>5</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>upper-class</t>
+          <t>higher-class</t>
         </is>
       </c>
       <c r="B11">
@@ -781,33 +749,30 @@
         <v>9</v>
       </c>
       <c r="E11">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F11">
-        <v>5</v>
-      </c>
-      <c r="G11">
-        <v>4</v>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>male</t>
-        </is>
+        <v>4</v>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>male</t>
+        </is>
+      </c>
+      <c r="H11">
+        <v>43</v>
       </c>
       <c r="I11">
-        <v>43</v>
+        <v>5</v>
       </c>
       <c r="J11">
-        <v>5</v>
-      </c>
-      <c r="K11">
         <v>5</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>upper-class</t>
+          <t>higher-class</t>
         </is>
       </c>
       <c r="B12">
@@ -820,33 +785,30 @@
         <v>9</v>
       </c>
       <c r="E12">
+        <v>3</v>
+      </c>
+      <c r="F12">
         <v>1</v>
       </c>
-      <c r="F12">
-        <v>3</v>
-      </c>
-      <c r="G12">
-        <v>2</v>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>male</t>
-        </is>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>male</t>
+        </is>
+      </c>
+      <c r="H12">
+        <v>37</v>
       </c>
       <c r="I12">
-        <v>37</v>
+        <v>4</v>
       </c>
       <c r="J12">
-        <v>4</v>
-      </c>
-      <c r="K12">
         <v>2</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>upper-class</t>
+          <t>higher-class</t>
         </is>
       </c>
       <c r="B13">
@@ -864,28 +826,25 @@
       <c r="F13">
         <v>4</v>
       </c>
-      <c r="G13">
-        <v>4</v>
-      </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>male</t>
-        </is>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>male</t>
+        </is>
+      </c>
+      <c r="H13">
+        <v>39</v>
       </c>
       <c r="I13">
-        <v>39</v>
+        <v>5</v>
       </c>
       <c r="J13">
-        <v>5</v>
-      </c>
-      <c r="K13">
         <v>8</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>upper-class</t>
+          <t>higher-class</t>
         </is>
       </c>
       <c r="B14">
@@ -901,30 +860,27 @@
         <v>4</v>
       </c>
       <c r="F14">
-        <v>4</v>
-      </c>
-      <c r="G14">
-        <v>4</v>
-      </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>male</t>
-        </is>
+        <v>3</v>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>male</t>
+        </is>
+      </c>
+      <c r="H14">
+        <v>39</v>
       </c>
       <c r="I14">
-        <v>39</v>
+        <v>6</v>
       </c>
       <c r="J14">
-        <v>6</v>
-      </c>
-      <c r="K14">
         <v>5</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>upper-class</t>
+          <t>higher-class</t>
         </is>
       </c>
       <c r="B15">
@@ -942,28 +898,25 @@
       <c r="F15">
         <v>4</v>
       </c>
-      <c r="G15">
-        <v>4</v>
-      </c>
-      <c r="H15" t="inlineStr">
-        <is>
-          <t>female</t>
-        </is>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>female</t>
+        </is>
+      </c>
+      <c r="H15">
+        <v>49</v>
       </c>
       <c r="I15">
-        <v>49</v>
+        <v>5</v>
       </c>
       <c r="J15">
-        <v>5</v>
-      </c>
-      <c r="K15">
         <v>7</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>upper-class</t>
+          <t>higher-class</t>
         </is>
       </c>
       <c r="B16">
@@ -979,30 +932,27 @@
         <v>4</v>
       </c>
       <c r="F16">
-        <v>4</v>
-      </c>
-      <c r="G16">
-        <v>4</v>
-      </c>
-      <c r="H16" t="inlineStr">
-        <is>
-          <t>female</t>
-        </is>
+        <v>3</v>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>female</t>
+        </is>
+      </c>
+      <c r="H16">
+        <v>56</v>
       </c>
       <c r="I16">
-        <v>56</v>
+        <v>4</v>
       </c>
       <c r="J16">
-        <v>4</v>
-      </c>
-      <c r="K16">
         <v>5</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>upper-class</t>
+          <t>higher-class</t>
         </is>
       </c>
       <c r="B17">
@@ -1020,28 +970,25 @@
       <c r="F17">
         <v>2</v>
       </c>
-      <c r="G17">
-        <v>3</v>
-      </c>
-      <c r="H17" t="inlineStr">
-        <is>
-          <t>female</t>
-        </is>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>female</t>
+        </is>
+      </c>
+      <c r="H17">
+        <v>43</v>
       </c>
       <c r="I17">
-        <v>43</v>
+        <v>5</v>
       </c>
       <c r="J17">
-        <v>5</v>
-      </c>
-      <c r="K17">
         <v>5</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>upper-class</t>
+          <t>higher-class</t>
         </is>
       </c>
       <c r="B18">
@@ -1057,30 +1004,27 @@
         <v>4</v>
       </c>
       <c r="F18">
-        <v>4</v>
-      </c>
-      <c r="G18">
-        <v>4</v>
-      </c>
-      <c r="H18" t="inlineStr">
-        <is>
-          <t>male</t>
-        </is>
+        <v>2</v>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>male</t>
+        </is>
+      </c>
+      <c r="H18">
+        <v>40</v>
       </c>
       <c r="I18">
-        <v>40</v>
+        <v>5</v>
       </c>
       <c r="J18">
-        <v>5</v>
-      </c>
-      <c r="K18">
         <v>3</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>upper-class</t>
+          <t>higher-class</t>
         </is>
       </c>
       <c r="B19">
@@ -1096,30 +1040,27 @@
         <v>3</v>
       </c>
       <c r="F19">
-        <v>3</v>
-      </c>
-      <c r="G19">
-        <v>2</v>
-      </c>
-      <c r="H19" t="inlineStr">
-        <is>
-          <t>female</t>
-        </is>
+        <v>4</v>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>female</t>
+        </is>
+      </c>
+      <c r="H19">
+        <v>43</v>
       </c>
       <c r="I19">
-        <v>43</v>
+        <v>6</v>
       </c>
       <c r="J19">
-        <v>6</v>
-      </c>
-      <c r="K19">
         <v>6</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>upper-class</t>
+          <t>higher-class</t>
         </is>
       </c>
       <c r="B20">
@@ -1137,28 +1078,25 @@
       <c r="F20">
         <v>3</v>
       </c>
-      <c r="G20">
-        <v>5</v>
-      </c>
-      <c r="H20" t="inlineStr">
-        <is>
-          <t>female</t>
-        </is>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>female</t>
+        </is>
+      </c>
+      <c r="H20">
+        <v>42</v>
       </c>
       <c r="I20">
-        <v>42</v>
+        <v>5</v>
       </c>
       <c r="J20">
-        <v>5</v>
-      </c>
-      <c r="K20">
         <v>3</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>upper-class</t>
+          <t>higher-class</t>
         </is>
       </c>
       <c r="B21">
@@ -1176,28 +1114,25 @@
       <c r="F21">
         <v>3</v>
       </c>
-      <c r="G21">
-        <v>4</v>
-      </c>
-      <c r="H21" t="inlineStr">
-        <is>
-          <t>female</t>
-        </is>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>female</t>
+        </is>
+      </c>
+      <c r="H21">
+        <v>50</v>
       </c>
       <c r="I21">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="J21">
-        <v>5</v>
-      </c>
-      <c r="K21">
         <v>4</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>upper-class</t>
+          <t>higher-class</t>
         </is>
       </c>
       <c r="B22">
@@ -1215,28 +1150,25 @@
       <c r="F22">
         <v>3</v>
       </c>
-      <c r="G22">
-        <v>4</v>
-      </c>
-      <c r="H22" t="inlineStr">
-        <is>
-          <t>male</t>
-        </is>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>male</t>
+        </is>
+      </c>
+      <c r="H22">
+        <v>46</v>
       </c>
       <c r="I22">
-        <v>46</v>
+        <v>5</v>
       </c>
       <c r="J22">
-        <v>5</v>
-      </c>
-      <c r="K22">
         <v>6</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>upper-class</t>
+          <t>higher-class</t>
         </is>
       </c>
       <c r="B23">
@@ -1252,30 +1184,27 @@
         <v>4</v>
       </c>
       <c r="F23">
-        <v>4</v>
-      </c>
-      <c r="G23">
-        <v>2</v>
-      </c>
-      <c r="H23" t="inlineStr">
-        <is>
-          <t>female</t>
-        </is>
+        <v>3</v>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>female</t>
+        </is>
+      </c>
+      <c r="H23">
+        <v>50</v>
       </c>
       <c r="I23">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="J23">
-        <v>6</v>
-      </c>
-      <c r="K23">
         <v>3</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>upper-class</t>
+          <t>higher-class</t>
         </is>
       </c>
       <c r="B24">
@@ -1291,30 +1220,27 @@
         <v>4</v>
       </c>
       <c r="F24">
-        <v>4</v>
-      </c>
-      <c r="G24">
-        <v>3</v>
-      </c>
-      <c r="H24" t="inlineStr">
-        <is>
-          <t>female</t>
-        </is>
+        <v>3</v>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>female</t>
+        </is>
+      </c>
+      <c r="H24">
+        <v>52</v>
       </c>
       <c r="I24">
-        <v>52</v>
+        <v>3</v>
       </c>
       <c r="J24">
-        <v>3</v>
-      </c>
-      <c r="K24">
         <v>5</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>upper-class</t>
+          <t>higher-class</t>
         </is>
       </c>
       <c r="B25">
@@ -1332,28 +1258,25 @@
       <c r="F25">
         <v>3</v>
       </c>
-      <c r="G25">
-        <v>3</v>
-      </c>
-      <c r="H25" t="inlineStr">
-        <is>
-          <t>female</t>
-        </is>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>female</t>
+        </is>
+      </c>
+      <c r="H25">
+        <v>40</v>
       </c>
       <c r="I25">
-        <v>40</v>
+        <v>6</v>
       </c>
       <c r="J25">
-        <v>6</v>
-      </c>
-      <c r="K25">
         <v>7</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>upper-class</t>
+          <t>higher-class</t>
         </is>
       </c>
       <c r="B26">
@@ -1366,33 +1289,30 @@
         <v>6</v>
       </c>
       <c r="E26">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F26">
-        <v>4</v>
-      </c>
-      <c r="G26">
-        <v>4</v>
-      </c>
-      <c r="H26" t="inlineStr">
-        <is>
-          <t>male</t>
-        </is>
+        <v>3</v>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>male</t>
+        </is>
+      </c>
+      <c r="H26">
+        <v>57</v>
       </c>
       <c r="I26">
-        <v>57</v>
+        <v>6</v>
       </c>
       <c r="J26">
-        <v>6</v>
-      </c>
-      <c r="K26">
         <v>3</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>upper-class</t>
+          <t>higher-class</t>
         </is>
       </c>
       <c r="B27">
@@ -1410,28 +1330,25 @@
       <c r="F27">
         <v>3</v>
       </c>
-      <c r="G27">
-        <v>4</v>
-      </c>
-      <c r="H27" t="inlineStr">
-        <is>
-          <t>female</t>
-        </is>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>female</t>
+        </is>
+      </c>
+      <c r="H27">
+        <v>41</v>
       </c>
       <c r="I27">
-        <v>41</v>
+        <v>5</v>
       </c>
       <c r="J27">
-        <v>5</v>
-      </c>
-      <c r="K27">
         <v>5</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>upper-class</t>
+          <t>higher-class</t>
         </is>
       </c>
       <c r="B28">
@@ -1449,28 +1366,25 @@
       <c r="F28">
         <v>3</v>
       </c>
-      <c r="G28">
-        <v>3</v>
-      </c>
-      <c r="H28" t="inlineStr">
-        <is>
-          <t>male</t>
-        </is>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>male</t>
+        </is>
+      </c>
+      <c r="H28">
+        <v>47</v>
       </c>
       <c r="I28">
-        <v>47</v>
+        <v>5</v>
       </c>
       <c r="J28">
-        <v>5</v>
-      </c>
-      <c r="K28">
         <v>2</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>upper-class</t>
+          <t>higher-class</t>
         </is>
       </c>
       <c r="B29">
@@ -1483,33 +1397,30 @@
         <v>6</v>
       </c>
       <c r="E29">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F29">
         <v>3</v>
       </c>
-      <c r="G29">
-        <v>3</v>
-      </c>
-      <c r="H29" t="inlineStr">
-        <is>
-          <t>male</t>
-        </is>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>male</t>
+        </is>
+      </c>
+      <c r="H29">
+        <v>40</v>
       </c>
       <c r="I29">
-        <v>40</v>
+        <v>4</v>
       </c>
       <c r="J29">
-        <v>4</v>
-      </c>
-      <c r="K29">
         <v>6</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>upper-class</t>
+          <t>higher-class</t>
         </is>
       </c>
       <c r="B30">
@@ -1527,28 +1438,25 @@
       <c r="F30">
         <v>4</v>
       </c>
-      <c r="G30">
-        <v>4</v>
-      </c>
-      <c r="H30" t="inlineStr">
-        <is>
-          <t>female</t>
-        </is>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>female</t>
+        </is>
+      </c>
+      <c r="H30">
+        <v>50</v>
       </c>
       <c r="I30">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="J30">
-        <v>5</v>
-      </c>
-      <c r="K30">
         <v>5</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>upper-class</t>
+          <t>higher-class</t>
         </is>
       </c>
       <c r="B31">
@@ -1564,23 +1472,20 @@
         <v>3</v>
       </c>
       <c r="F31">
-        <v>3</v>
-      </c>
-      <c r="G31">
-        <v>4</v>
-      </c>
-      <c r="H31" t="inlineStr">
-        <is>
-          <t>female</t>
-        </is>
+        <v>4</v>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>female</t>
+        </is>
+      </c>
+      <c r="H31">
+        <v>59</v>
       </c>
       <c r="I31">
-        <v>59</v>
+        <v>5</v>
       </c>
       <c r="J31">
-        <v>5</v>
-      </c>
-      <c r="K31">
         <v>5</v>
       </c>
     </row>
@@ -1605,21 +1510,18 @@
       <c r="F32">
         <v>4</v>
       </c>
-      <c r="G32">
-        <v>4</v>
-      </c>
-      <c r="H32" t="inlineStr">
-        <is>
-          <t>male</t>
-        </is>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>male</t>
+        </is>
+      </c>
+      <c r="H32">
+        <v>54</v>
       </c>
       <c r="I32">
-        <v>54</v>
+        <v>5</v>
       </c>
       <c r="J32">
-        <v>5</v>
-      </c>
-      <c r="K32">
         <v>7</v>
       </c>
     </row>
@@ -1642,23 +1544,20 @@
         <v>3</v>
       </c>
       <c r="F33">
-        <v>3</v>
-      </c>
-      <c r="G33">
-        <v>4</v>
-      </c>
-      <c r="H33" t="inlineStr">
-        <is>
-          <t>male</t>
-        </is>
+        <v>4</v>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>male</t>
+        </is>
+      </c>
+      <c r="H33">
+        <v>52</v>
       </c>
       <c r="I33">
-        <v>52</v>
+        <v>4</v>
       </c>
       <c r="J33">
-        <v>4</v>
-      </c>
-      <c r="K33">
         <v>7</v>
       </c>
     </row>
@@ -1683,21 +1582,18 @@
       <c r="F34">
         <v>3</v>
       </c>
-      <c r="G34">
-        <v>3</v>
-      </c>
-      <c r="H34" t="inlineStr">
-        <is>
-          <t>female</t>
-        </is>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>female</t>
+        </is>
+      </c>
+      <c r="H34">
+        <v>41</v>
       </c>
       <c r="I34">
-        <v>41</v>
+        <v>5</v>
       </c>
       <c r="J34">
-        <v>5</v>
-      </c>
-      <c r="K34">
         <v>6</v>
       </c>
     </row>
@@ -1720,23 +1616,20 @@
         <v>3</v>
       </c>
       <c r="F35">
-        <v>3</v>
-      </c>
-      <c r="G35">
-        <v>3</v>
-      </c>
-      <c r="H35" t="inlineStr">
-        <is>
-          <t>male</t>
-        </is>
+        <v>4</v>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>male</t>
+        </is>
+      </c>
+      <c r="H35">
+        <v>51</v>
       </c>
       <c r="I35">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="J35">
-        <v>6</v>
-      </c>
-      <c r="K35">
         <v>9</v>
       </c>
     </row>
@@ -1761,21 +1654,18 @@
       <c r="F36">
         <v>2</v>
       </c>
-      <c r="G36">
-        <v>3</v>
-      </c>
-      <c r="H36" t="inlineStr">
-        <is>
-          <t>female</t>
-        </is>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>female</t>
+        </is>
+      </c>
+      <c r="H36">
+        <v>38</v>
       </c>
       <c r="I36">
-        <v>38</v>
+        <v>4</v>
       </c>
       <c r="J36">
-        <v>4</v>
-      </c>
-      <c r="K36">
         <v>5</v>
       </c>
     </row>
@@ -1798,23 +1688,20 @@
         <v>3</v>
       </c>
       <c r="F37">
-        <v>3</v>
-      </c>
-      <c r="G37">
-        <v>4</v>
-      </c>
-      <c r="H37" t="inlineStr">
-        <is>
-          <t>female</t>
-        </is>
+        <v>4</v>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>female</t>
+        </is>
+      </c>
+      <c r="H37">
+        <v>39</v>
       </c>
       <c r="I37">
-        <v>39</v>
+        <v>4</v>
       </c>
       <c r="J37">
-        <v>4</v>
-      </c>
-      <c r="K37">
         <v>4</v>
       </c>
     </row>
@@ -1839,21 +1726,18 @@
       <c r="F38">
         <v>3</v>
       </c>
-      <c r="G38">
-        <v>4</v>
-      </c>
-      <c r="H38" t="inlineStr">
-        <is>
-          <t>female</t>
-        </is>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>female</t>
+        </is>
+      </c>
+      <c r="H38">
+        <v>47</v>
       </c>
       <c r="I38">
-        <v>47</v>
+        <v>3</v>
       </c>
       <c r="J38">
-        <v>3</v>
-      </c>
-      <c r="K38">
         <v>4</v>
       </c>
     </row>
@@ -1878,21 +1762,18 @@
       <c r="F39">
         <v>4</v>
       </c>
-      <c r="G39">
-        <v>3</v>
-      </c>
-      <c r="H39" t="inlineStr">
-        <is>
-          <t>female</t>
-        </is>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>female</t>
+        </is>
+      </c>
+      <c r="H39">
+        <v>50</v>
       </c>
       <c r="I39">
-        <v>50</v>
+        <v>4</v>
       </c>
       <c r="J39">
-        <v>4</v>
-      </c>
-      <c r="K39">
         <v>6</v>
       </c>
     </row>
@@ -1917,21 +1798,18 @@
       <c r="F40">
         <v>3</v>
       </c>
-      <c r="G40">
-        <v>3</v>
-      </c>
-      <c r="H40" t="inlineStr">
-        <is>
-          <t>female</t>
-        </is>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>female</t>
+        </is>
+      </c>
+      <c r="H40">
+        <v>54</v>
       </c>
       <c r="I40">
-        <v>54</v>
+        <v>4</v>
       </c>
       <c r="J40">
-        <v>4</v>
-      </c>
-      <c r="K40">
         <v>7</v>
       </c>
     </row>
@@ -1954,23 +1832,20 @@
         <v>3</v>
       </c>
       <c r="F41">
-        <v>3</v>
-      </c>
-      <c r="G41">
-        <v>3</v>
-      </c>
-      <c r="H41" t="inlineStr">
-        <is>
-          <t>male</t>
-        </is>
+        <v>2</v>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>male</t>
+        </is>
+      </c>
+      <c r="H41">
+        <v>58</v>
       </c>
       <c r="I41">
-        <v>58</v>
+        <v>4</v>
       </c>
       <c r="J41">
-        <v>4</v>
-      </c>
-      <c r="K41">
         <v>2</v>
       </c>
     </row>
@@ -1990,26 +1865,23 @@
         <v>4</v>
       </c>
       <c r="E42">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F42">
         <v>3</v>
       </c>
-      <c r="G42">
-        <v>3</v>
-      </c>
-      <c r="H42" t="inlineStr">
-        <is>
-          <t>female</t>
-        </is>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>female</t>
+        </is>
+      </c>
+      <c r="H42">
+        <v>46</v>
       </c>
       <c r="I42">
-        <v>46</v>
+        <v>4</v>
       </c>
       <c r="J42">
-        <v>4</v>
-      </c>
-      <c r="K42">
         <v>4</v>
       </c>
     </row>
@@ -2029,26 +1901,23 @@
         <v>6</v>
       </c>
       <c r="E43">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F43">
-        <v>5</v>
-      </c>
-      <c r="G43">
-        <v>4</v>
-      </c>
-      <c r="H43" t="inlineStr">
-        <is>
-          <t>female</t>
-        </is>
+        <v>4</v>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>female</t>
+        </is>
+      </c>
+      <c r="H43">
+        <v>52</v>
       </c>
       <c r="I43">
-        <v>52</v>
+        <v>3</v>
       </c>
       <c r="J43">
-        <v>3</v>
-      </c>
-      <c r="K43">
         <v>3</v>
       </c>
     </row>
@@ -2068,26 +1937,23 @@
         <v>6</v>
       </c>
       <c r="E44">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F44">
-        <v>4</v>
-      </c>
-      <c r="G44">
-        <v>3</v>
-      </c>
-      <c r="H44" t="inlineStr">
-        <is>
-          <t>female</t>
-        </is>
+        <v>3</v>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>female</t>
+        </is>
+      </c>
+      <c r="H44">
+        <v>37</v>
       </c>
       <c r="I44">
-        <v>37</v>
+        <v>5</v>
       </c>
       <c r="J44">
-        <v>5</v>
-      </c>
-      <c r="K44">
         <v>6</v>
       </c>
     </row>
@@ -2110,23 +1976,20 @@
         <v>3</v>
       </c>
       <c r="F45">
-        <v>3</v>
-      </c>
-      <c r="G45">
-        <v>2</v>
-      </c>
-      <c r="H45" t="inlineStr">
-        <is>
-          <t>female</t>
-        </is>
+        <v>2</v>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>female</t>
+        </is>
+      </c>
+      <c r="H45">
+        <v>55</v>
       </c>
       <c r="I45">
-        <v>55</v>
+        <v>3</v>
       </c>
       <c r="J45">
-        <v>3</v>
-      </c>
-      <c r="K45">
         <v>5</v>
       </c>
     </row>
@@ -2151,21 +2014,18 @@
       <c r="F46">
         <v>4</v>
       </c>
-      <c r="G46">
-        <v>4</v>
-      </c>
-      <c r="H46" t="inlineStr">
-        <is>
-          <t>female</t>
-        </is>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>female</t>
+        </is>
+      </c>
+      <c r="H46">
+        <v>50</v>
       </c>
       <c r="I46">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="J46">
-        <v>5</v>
-      </c>
-      <c r="K46">
         <v>4</v>
       </c>
     </row>
@@ -2185,26 +2045,23 @@
         <v>4</v>
       </c>
       <c r="E47">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F47">
         <v>3</v>
       </c>
-      <c r="G47">
-        <v>4</v>
-      </c>
-      <c r="H47" t="inlineStr">
-        <is>
-          <t>female</t>
-        </is>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>female</t>
+        </is>
+      </c>
+      <c r="H47">
+        <v>50</v>
       </c>
       <c r="I47">
-        <v>50</v>
+        <v>4</v>
       </c>
       <c r="J47">
-        <v>4</v>
-      </c>
-      <c r="K47">
         <v>5</v>
       </c>
     </row>
@@ -2224,26 +2081,23 @@
         <v>2</v>
       </c>
       <c r="E48">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F48">
         <v>3</v>
       </c>
-      <c r="G48">
-        <v>4</v>
-      </c>
-      <c r="H48" t="inlineStr">
-        <is>
-          <t>male</t>
-        </is>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>male</t>
+        </is>
+      </c>
+      <c r="H48">
+        <v>37</v>
       </c>
       <c r="I48">
-        <v>37</v>
+        <v>3</v>
       </c>
       <c r="J48">
-        <v>3</v>
-      </c>
-      <c r="K48">
         <v>3</v>
       </c>
     </row>
@@ -2268,21 +2122,18 @@
       <c r="F49">
         <v>2</v>
       </c>
-      <c r="G49">
-        <v>2</v>
-      </c>
-      <c r="H49" t="inlineStr">
-        <is>
-          <t>male</t>
-        </is>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>male</t>
+        </is>
+      </c>
+      <c r="H49">
+        <v>42</v>
       </c>
       <c r="I49">
-        <v>42</v>
+        <v>4</v>
       </c>
       <c r="J49">
-        <v>4</v>
-      </c>
-      <c r="K49">
         <v>5</v>
       </c>
     </row>
@@ -2307,21 +2158,18 @@
       <c r="F50">
         <v>3</v>
       </c>
-      <c r="G50">
-        <v>3</v>
-      </c>
-      <c r="H50" t="inlineStr">
-        <is>
-          <t>male</t>
-        </is>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>male</t>
+        </is>
+      </c>
+      <c r="H50">
+        <v>39</v>
       </c>
       <c r="I50">
-        <v>39</v>
+        <v>4</v>
       </c>
       <c r="J50">
-        <v>4</v>
-      </c>
-      <c r="K50">
         <v>3</v>
       </c>
     </row>
@@ -2346,21 +2194,18 @@
       <c r="F51">
         <v>3</v>
       </c>
-      <c r="G51">
-        <v>4</v>
-      </c>
-      <c r="H51" t="inlineStr">
-        <is>
-          <t>female</t>
-        </is>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>female</t>
+        </is>
+      </c>
+      <c r="H51">
+        <v>42</v>
       </c>
       <c r="I51">
-        <v>42</v>
+        <v>5</v>
       </c>
       <c r="J51">
-        <v>5</v>
-      </c>
-      <c r="K51">
         <v>3</v>
       </c>
     </row>
@@ -2385,21 +2230,18 @@
       <c r="F52">
         <v>3</v>
       </c>
-      <c r="G52">
-        <v>2</v>
-      </c>
-      <c r="H52" t="inlineStr">
-        <is>
-          <t>female</t>
-        </is>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>female</t>
+        </is>
+      </c>
+      <c r="H52">
+        <v>44</v>
       </c>
       <c r="I52">
-        <v>44</v>
+        <v>5</v>
       </c>
       <c r="J52">
-        <v>5</v>
-      </c>
-      <c r="K52">
         <v>6</v>
       </c>
     </row>
@@ -2419,26 +2261,23 @@
         <v>5</v>
       </c>
       <c r="E53">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F53">
         <v>2</v>
       </c>
-      <c r="G53">
-        <v>3</v>
-      </c>
-      <c r="H53" t="inlineStr">
-        <is>
-          <t>female</t>
-        </is>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>female</t>
+        </is>
+      </c>
+      <c r="H53">
+        <v>46</v>
       </c>
       <c r="I53">
-        <v>46</v>
+        <v>5</v>
       </c>
       <c r="J53">
-        <v>5</v>
-      </c>
-      <c r="K53">
         <v>5</v>
       </c>
     </row>
@@ -2458,26 +2297,23 @@
         <v>5</v>
       </c>
       <c r="E54">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F54">
-        <v>2</v>
-      </c>
-      <c r="G54">
-        <v>3</v>
-      </c>
-      <c r="H54" t="inlineStr">
-        <is>
-          <t>male</t>
-        </is>
+        <v>4</v>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>male</t>
+        </is>
+      </c>
+      <c r="H54">
+        <v>49</v>
       </c>
       <c r="I54">
-        <v>49</v>
+        <v>3</v>
       </c>
       <c r="J54">
-        <v>3</v>
-      </c>
-      <c r="K54">
         <v>3</v>
       </c>
     </row>
@@ -2497,26 +2333,23 @@
         <v>6</v>
       </c>
       <c r="E55">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F55">
         <v>4</v>
       </c>
-      <c r="G55">
-        <v>4</v>
-      </c>
-      <c r="H55" t="inlineStr">
-        <is>
-          <t>male</t>
-        </is>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>male</t>
+        </is>
+      </c>
+      <c r="H55">
+        <v>45</v>
       </c>
       <c r="I55">
-        <v>45</v>
+        <v>4</v>
       </c>
       <c r="J55">
-        <v>4</v>
-      </c>
-      <c r="K55">
         <v>6</v>
       </c>
     </row>
@@ -2536,26 +2369,23 @@
         <v>5</v>
       </c>
       <c r="E56">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F56">
-        <v>3</v>
-      </c>
-      <c r="G56">
-        <v>4</v>
-      </c>
-      <c r="H56" t="inlineStr">
-        <is>
-          <t>female</t>
-        </is>
+        <v>4</v>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>female</t>
+        </is>
+      </c>
+      <c r="H56">
+        <v>44</v>
       </c>
       <c r="I56">
-        <v>44</v>
+        <v>5</v>
       </c>
       <c r="J56">
-        <v>5</v>
-      </c>
-      <c r="K56">
         <v>5</v>
       </c>
     </row>
@@ -2578,23 +2408,20 @@
         <v>3</v>
       </c>
       <c r="F57">
-        <v>3</v>
-      </c>
-      <c r="G57">
-        <v>3</v>
-      </c>
-      <c r="H57" t="inlineStr">
-        <is>
-          <t>male</t>
-        </is>
+        <v>4</v>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>male</t>
+        </is>
+      </c>
+      <c r="H57">
+        <v>40</v>
       </c>
       <c r="I57">
-        <v>40</v>
+        <v>5</v>
       </c>
       <c r="J57">
-        <v>5</v>
-      </c>
-      <c r="K57">
         <v>5</v>
       </c>
     </row>
@@ -2617,23 +2444,20 @@
         <v>4</v>
       </c>
       <c r="F58">
-        <v>4</v>
-      </c>
-      <c r="G58">
-        <v>4</v>
-      </c>
-      <c r="H58" t="inlineStr">
-        <is>
-          <t>female</t>
-        </is>
+        <v>3</v>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>female</t>
+        </is>
+      </c>
+      <c r="H58">
+        <v>40</v>
       </c>
       <c r="I58">
-        <v>40</v>
+        <v>3</v>
       </c>
       <c r="J58">
-        <v>3</v>
-      </c>
-      <c r="K58">
         <v>5</v>
       </c>
     </row>
@@ -2658,21 +2482,18 @@
       <c r="F59">
         <v>3</v>
       </c>
-      <c r="G59">
-        <v>4</v>
-      </c>
-      <c r="H59" t="inlineStr">
-        <is>
-          <t>male</t>
-        </is>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>male</t>
+        </is>
+      </c>
+      <c r="H59">
+        <v>51</v>
       </c>
       <c r="I59">
-        <v>51</v>
+        <v>4</v>
       </c>
       <c r="J59">
-        <v>4</v>
-      </c>
-      <c r="K59">
         <v>5</v>
       </c>
     </row>
@@ -2692,26 +2513,23 @@
         <v>10</v>
       </c>
       <c r="E60">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F60">
-        <v>2</v>
-      </c>
-      <c r="G60">
-        <v>3</v>
-      </c>
-      <c r="H60" t="inlineStr">
-        <is>
-          <t>female</t>
-        </is>
+        <v>3</v>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>female</t>
+        </is>
+      </c>
+      <c r="H60">
+        <v>42</v>
       </c>
       <c r="I60">
-        <v>42</v>
+        <v>4</v>
       </c>
       <c r="J60">
-        <v>4</v>
-      </c>
-      <c r="K60">
         <v>10</v>
       </c>
     </row>
@@ -2736,21 +2554,18 @@
       <c r="F61">
         <v>1</v>
       </c>
-      <c r="G61">
-        <v>1</v>
-      </c>
-      <c r="H61" t="inlineStr">
-        <is>
-          <t>male</t>
-        </is>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>male</t>
+        </is>
+      </c>
+      <c r="H61">
+        <v>40</v>
       </c>
       <c r="I61">
-        <v>40</v>
+        <v>4</v>
       </c>
       <c r="J61">
-        <v>4</v>
-      </c>
-      <c r="K61">
         <v>4</v>
       </c>
     </row>
@@ -2770,26 +2585,23 @@
         <v>4</v>
       </c>
       <c r="E62">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F62">
-        <v>4</v>
-      </c>
-      <c r="G62">
-        <v>3</v>
-      </c>
-      <c r="H62" t="inlineStr">
-        <is>
-          <t>male</t>
-        </is>
+        <v>3</v>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>male</t>
+        </is>
+      </c>
+      <c r="H62">
+        <v>47</v>
       </c>
       <c r="I62">
-        <v>47</v>
+        <v>5</v>
       </c>
       <c r="J62">
-        <v>5</v>
-      </c>
-      <c r="K62">
         <v>2</v>
       </c>
     </row>
@@ -2814,21 +2626,18 @@
       <c r="F63">
         <v>3</v>
       </c>
-      <c r="G63">
-        <v>3</v>
-      </c>
-      <c r="H63" t="inlineStr">
-        <is>
-          <t>male</t>
-        </is>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>male</t>
+        </is>
+      </c>
+      <c r="H63">
+        <v>40</v>
       </c>
       <c r="I63">
-        <v>40</v>
+        <v>4</v>
       </c>
       <c r="J63">
-        <v>4</v>
-      </c>
-      <c r="K63">
         <v>5</v>
       </c>
     </row>
@@ -2851,23 +2660,20 @@
         <v>3</v>
       </c>
       <c r="F64">
-        <v>3</v>
-      </c>
-      <c r="G64">
-        <v>2</v>
-      </c>
-      <c r="H64" t="inlineStr">
-        <is>
-          <t>female</t>
-        </is>
+        <v>2</v>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>female</t>
+        </is>
+      </c>
+      <c r="H64">
+        <v>42</v>
       </c>
       <c r="I64">
-        <v>42</v>
+        <v>6</v>
       </c>
       <c r="J64">
-        <v>6</v>
-      </c>
-      <c r="K64">
         <v>5</v>
       </c>
     </row>
@@ -2892,21 +2698,18 @@
       <c r="F65">
         <v>3</v>
       </c>
-      <c r="G65">
-        <v>4</v>
-      </c>
-      <c r="H65" t="inlineStr">
-        <is>
-          <t>male</t>
-        </is>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>male</t>
+        </is>
+      </c>
+      <c r="H65">
+        <v>50</v>
       </c>
       <c r="I65">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="J65">
-        <v>5</v>
-      </c>
-      <c r="K65">
         <v>5</v>
       </c>
     </row>
@@ -2929,23 +2732,20 @@
         <v>3</v>
       </c>
       <c r="F66">
-        <v>3</v>
-      </c>
-      <c r="G66">
-        <v>2</v>
-      </c>
-      <c r="H66" t="inlineStr">
-        <is>
-          <t>male</t>
-        </is>
+        <v>2</v>
+      </c>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t>male</t>
+        </is>
+      </c>
+      <c r="H66">
+        <v>50</v>
       </c>
       <c r="I66">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="J66">
-        <v>5</v>
-      </c>
-      <c r="K66">
         <v>7</v>
       </c>
     </row>
@@ -2968,23 +2768,20 @@
         <v>3</v>
       </c>
       <c r="F67">
-        <v>3</v>
-      </c>
-      <c r="G67">
-        <v>4</v>
-      </c>
-      <c r="H67" t="inlineStr">
-        <is>
-          <t>female</t>
-        </is>
+        <v>4</v>
+      </c>
+      <c r="G67" t="inlineStr">
+        <is>
+          <t>female</t>
+        </is>
+      </c>
+      <c r="H67">
+        <v>53</v>
       </c>
       <c r="I67">
-        <v>53</v>
+        <v>5</v>
       </c>
       <c r="J67">
-        <v>5</v>
-      </c>
-      <c r="K67">
         <v>5</v>
       </c>
     </row>

</xml_diff>